<commit_message>
Adding more to tidy data import
</commit_message>
<xml_diff>
--- a/posts/S07E10_tidy_05/data/students.xlsx
+++ b/posts/S07E10_tidy_05/data/students.xlsx
@@ -1,8 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27514"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://buckeyemailosu-my.sharepoint.com/personal/cooperstone_1_osu_edu/Documents/BuckeyeBox Data/JLC_Files/OSU/research/code club/osu-codeclub.github.io/posts/S07E10_tidy_05/data/"/>
@@ -16,7 +16,7 @@
     <sheet name="students" sheetId="1" r:id="rId1"/>
     <sheet name="students_2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -103,7 +103,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -474,9 +474,9 @@
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.95"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -493,7 +493,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5">
       <c r="A2">
         <v>1</v>
       </c>
@@ -510,7 +510,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5">
       <c r="A3">
         <v>2</v>
       </c>
@@ -527,7 +527,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5">
       <c r="A4">
         <v>3</v>
       </c>
@@ -544,7 +544,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5">
       <c r="A5">
         <v>4</v>
       </c>
@@ -558,7 +558,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5">
       <c r="A6">
         <v>5</v>
       </c>
@@ -575,7 +575,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5">
       <c r="A7">
         <v>6</v>
       </c>
@@ -605,9 +605,9 @@
       <selection activeCell="B18" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.95"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -624,7 +624,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5">
       <c r="A2">
         <v>1</v>
       </c>
@@ -641,7 +641,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5">
       <c r="A3">
         <v>2</v>
       </c>
@@ -658,7 +658,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5">
       <c r="A4">
         <v>3</v>
       </c>
@@ -675,7 +675,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5">
       <c r="A5">
         <v>4</v>
       </c>
@@ -689,7 +689,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5">
       <c r="A6">
         <v>5</v>
       </c>
@@ -706,7 +706,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5">
       <c r="A7">
         <v>6</v>
       </c>

</xml_diff>